<commit_message>
FME feature of intrest change
</commit_message>
<xml_diff>
--- a/FME_data_in/KalasatamaCityGML.xlsx
+++ b/FME_data_in/KalasatamaCityGML.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="63">
   <si>
     <t>gml_id</t>
   </si>
@@ -194,6 +194,12 @@
   </si>
   <si>
     <t>BID_fcdec70c-ff33-4849-b60e-acd58112f7e4</t>
+  </si>
+  <si>
+    <t>BID_04b55dd6-c136-49a6-b142-723c0eb5ee89</t>
+  </si>
+  <si>
+    <t>BID_059d0a21-a2a7-4aa5-b427-2975517f09ba</t>
   </si>
 </sst>
 </file>
@@ -981,6 +987,102 @@
         <v>811.0</v>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B65" s="2">
+        <v>834.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B66" s="2">
+        <v>833.0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B67" s="2">
+        <v>832.0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B68" s="2">
+        <v>831.0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B69" s="2">
+        <v>830.0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B70" s="2">
+        <v>829.0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B71" s="2">
+        <v>828.0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B72" s="2">
+        <v>820.0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B73" s="2">
+        <v>821.0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B74" s="2">
+        <v>822.0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B75" s="2">
+        <v>823.0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B76" s="2">
+        <v>826.0</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>